<commit_message>
Final de Admon Inicio de Operaciones
</commit_message>
<xml_diff>
--- a/Semestre 2/Administración y Valoración Financiera/2-MODELO VALORACIÓN_TAB Estudiantes v.+cuentas - SIMPLIFICADO.xlsx
+++ b/Semestre 2/Administración y Valoración Financiera/2-MODELO VALORACIÓN_TAB Estudiantes v.+cuentas - SIMPLIFICADO.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NIGOJ\OneDrive\Desktop\NICO\MAF\Semestre 2\Administración y Valoración Financiera\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47328FBE-32FF-4C26-A690-F255ACBD8F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7540FFA6-48CD-4E01-86DC-AAFEEB8FED7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MODELO VALORACIÓN SIMPLIFICADO" sheetId="15" r:id="rId1"/>
+    <sheet name="KPI's" sheetId="16" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'MODELO VALORACIÓN SIMPLIFICADO'!#REF!</definedName>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="254">
   <si>
     <t>VENTAS</t>
   </si>
@@ -1133,13 +1134,155 @@
   <si>
     <t>EV</t>
   </si>
+  <si>
+    <t>Margen EBITDA</t>
+  </si>
+  <si>
+    <t>RSP</t>
+  </si>
+  <si>
+    <t>UODI/INOPdi</t>
+  </si>
+  <si>
+    <t>ROIC</t>
+  </si>
+  <si>
+    <t>D/(E+D)</t>
+  </si>
+  <si>
+    <t>E/(E+D)</t>
+  </si>
+  <si>
+    <t>Libre Riesgo</t>
+  </si>
+  <si>
+    <t>Prima de Riesgo</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Riesgo País</t>
+  </si>
+  <si>
+    <t>Ke</t>
+  </si>
+  <si>
+    <t>Kd</t>
+  </si>
+  <si>
+    <t>Ventas</t>
+  </si>
+  <si>
+    <t>EVA NO Operativo</t>
+  </si>
+  <si>
+    <t>EVA TOTAL</t>
+  </si>
+  <si>
+    <t>Margen EVA</t>
+  </si>
+  <si>
+    <t>Crecimiento en Ventas</t>
+  </si>
+  <si>
+    <t>EVA Momentum</t>
+  </si>
+  <si>
+    <t>Crecimiento Rentable</t>
+  </si>
+  <si>
+    <t>Ganancia en Productividad</t>
+  </si>
+  <si>
+    <t>Tasa de Crecimiento Sostenible</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>ROE</t>
+  </si>
+  <si>
+    <t>Utilización de los activos fijos</t>
+  </si>
+  <si>
+    <t>Variable de ajuste del modelo de planeación financiera???? (Plug)</t>
+  </si>
+  <si>
+    <t>EBITDAC</t>
+  </si>
+  <si>
+    <t>Rentabilidad sobre el PATRIMONIO</t>
+  </si>
+  <si>
+    <t>Tasa de crecimiento sostenible de la EMPRESA</t>
+  </si>
+  <si>
+    <t>EVA operativo, no operativo y total</t>
+  </si>
+  <si>
+    <t>EVA momentum (discriminado en ganancia en productividad y crecimiento rentable)</t>
+  </si>
+  <si>
+    <t>UODI / INOPdi</t>
+  </si>
+  <si>
+    <t>Ventas de equilibrio (podríamos sacarle una gráfica como en clase)</t>
+  </si>
+  <si>
+    <t>Capital empleado fijo y Variable</t>
+  </si>
+  <si>
+    <t>Utilidad mínima requerida</t>
+  </si>
+  <si>
+    <t>Puntos de equilibrio operativo y económico</t>
+  </si>
+  <si>
+    <t>Margenes de seguridad operativo y económico</t>
+  </si>
+  <si>
+    <t>PE-EBITDA=CF-D&amp;A/indice de contribución</t>
+  </si>
+  <si>
+    <t>Poner explícita la estructura de Capital</t>
+  </si>
+  <si>
+    <t>Ke y Kd</t>
+  </si>
+  <si>
+    <t>Múltiplos de salida (EV/EBITDA....)</t>
+  </si>
+  <si>
+    <t>2023P</t>
+  </si>
+  <si>
+    <t>Var</t>
+  </si>
+  <si>
+    <t>Participación</t>
+  </si>
+  <si>
+    <t>Razón de Intensidad del Capital</t>
+  </si>
+  <si>
+    <t>Tasa de Crecimiento Interno</t>
+  </si>
+  <si>
+    <t>ROA</t>
+  </si>
+  <si>
+    <t>Estructura de Capital</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="13">
+  <numFmts count="15">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -1151,7 +1294,8 @@
     <numFmt numFmtId="171" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="172" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="173" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;?_-;_-@_-"/>
-    <numFmt numFmtId="175" formatCode="0.0\x"/>
+    <numFmt numFmtId="174" formatCode="0.0\x"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="27" x14ac:knownFonts="1">
     <font>
@@ -1337,7 +1481,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1395,6 +1539,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1483,7 +1633,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1505,8 +1655,9 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1646,12 +1797,12 @@
     <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="9" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="9" applyFont="1"/>
-    <xf numFmtId="175" fontId="24" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="24" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="172" fontId="23" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="23" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="24" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="174" fontId="23" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="174" fontId="24" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="172" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1726,8 +1877,21 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="11" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="22">
     <cellStyle name="Comma [0] 2" xfId="13" xr:uid="{CC363B22-EE3C-4062-AB65-F428CFAE3412}"/>
     <cellStyle name="Comma [0] 2 2" xfId="18" xr:uid="{CDABCF41-4F22-404C-8877-13FF3B5966BC}"/>
     <cellStyle name="Comma 2" xfId="10" xr:uid="{B9EC1A25-925A-45A7-83CB-4F3E214EC30D}"/>
@@ -1735,6 +1899,7 @@
     <cellStyle name="Millares [0]" xfId="2" builtinId="6"/>
     <cellStyle name="Millares [0] 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Millares 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Moneda" xfId="21" builtinId="4"/>
     <cellStyle name="Moneda 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -4035,15 +4200,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>22860</xdr:colOff>
+          <xdr:colOff>19050</xdr:colOff>
           <xdr:row>43</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>11</xdr:col>
-          <xdr:colOff>1104900</xdr:colOff>
+          <xdr:col>12</xdr:col>
+          <xdr:colOff>3175</xdr:colOff>
           <xdr:row>44</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4093,15 +4258,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>617220</xdr:colOff>
+          <xdr:colOff>619125</xdr:colOff>
           <xdr:row>189</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
-          <xdr:row>190</xdr:row>
-          <xdr:rowOff>198120</xdr:rowOff>
+          <xdr:colOff>476250</xdr:colOff>
+          <xdr:row>191</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4475,26 +4640,26 @@
   </sheetPr>
   <dimension ref="A1:S340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A295" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="A55" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B318" sqref="B318"/>
+      <selection pane="topRight" activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.23046875" defaultRowHeight="16.2" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.19921875" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="48.3046875" customWidth="1"/>
-    <col min="2" max="2" width="12.23046875" customWidth="1"/>
-    <col min="3" max="3" width="12.3828125" customWidth="1"/>
-    <col min="4" max="4" width="12.3046875" customWidth="1"/>
-    <col min="5" max="5" width="12.07421875" customWidth="1"/>
-    <col min="6" max="6" width="12.23046875" customWidth="1"/>
-    <col min="7" max="7" width="13.23046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.3046875" customWidth="1"/>
-    <col min="10" max="10" width="32.4609375" customWidth="1"/>
-    <col min="14" max="14" width="8.765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.296875" customWidth="1"/>
+    <col min="2" max="2" width="12.19921875" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" customWidth="1"/>
+    <col min="4" max="4" width="12.296875" customWidth="1"/>
+    <col min="5" max="5" width="12.09765625" customWidth="1"/>
+    <col min="6" max="6" width="12.19921875" customWidth="1"/>
+    <col min="7" max="7" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.296875" customWidth="1"/>
+    <col min="10" max="10" width="32.5" customWidth="1"/>
+    <col min="14" max="14" width="8.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
         <v>83</v>
       </c>
@@ -4506,8 +4671,8 @@
       <c r="G1" s="39"/>
       <c r="H1" s="39"/>
     </row>
-    <row r="2" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -4538,7 +4703,7 @@
       <c r="N3" s="149"/>
       <c r="O3" s="149"/>
     </row>
-    <row r="4" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="J4" s="122" t="s">
@@ -4560,7 +4725,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="5" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A5" s="139" t="s">
         <v>19</v>
       </c>
@@ -4607,7 +4772,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="6" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -4647,7 +4812,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A7" s="139" t="s">
         <v>1</v>
       </c>
@@ -4694,7 +4859,7 @@
         <v>84000</v>
       </c>
     </row>
-    <row r="8" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -4736,7 +4901,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -4778,7 +4943,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="10" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -4820,7 +4985,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -4860,7 +5025,7 @@
         <v>453150.4581090695</v>
       </c>
     </row>
-    <row r="12" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -4900,7 +5065,7 @@
         <v>34000</v>
       </c>
     </row>
-    <row r="13" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -4942,7 +5107,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="14" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -4971,7 +5136,7 @@
       <c r="N14" s="130"/>
       <c r="O14" s="130"/>
     </row>
-    <row r="15" spans="1:15" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A15" s="139" t="s">
         <v>3</v>
       </c>
@@ -5007,7 +5172,7 @@
       <c r="N15" s="150"/>
       <c r="O15" s="150"/>
     </row>
-    <row r="16" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>158</v>
       </c>
@@ -5036,7 +5201,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="17" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>159</v>
       </c>
@@ -5066,7 +5231,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="18" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -5108,7 +5273,7 @@
         <v>0.30999999999999994</v>
       </c>
     </row>
-    <row r="19" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A19" s="139" t="s">
         <v>26</v>
       </c>
@@ -5155,7 +5320,7 @@
         <v>84000</v>
       </c>
     </row>
-    <row r="20" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A20" s="139" t="s">
         <v>27</v>
       </c>
@@ -5202,7 +5367,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>160</v>
       </c>
@@ -5232,7 +5397,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="22" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A22" s="139" t="s">
         <v>28</v>
       </c>
@@ -5279,7 +5444,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>161</v>
       </c>
@@ -5309,7 +5474,7 @@
         <v>453150.42166893516</v>
       </c>
     </row>
-    <row r="24" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A24" s="139" t="s">
         <v>29</v>
       </c>
@@ -5356,7 +5521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>162</v>
       </c>
@@ -5386,7 +5551,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="26" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A26" s="139" t="s">
         <v>30</v>
       </c>
@@ -5420,7 +5585,7 @@
       <c r="N26" s="133"/>
       <c r="O26" s="133"/>
     </row>
-    <row r="27" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>163</v>
       </c>
@@ -5439,7 +5604,7 @@
       <c r="N27" s="149"/>
       <c r="O27" s="149"/>
     </row>
-    <row r="28" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A28" s="139" t="s">
         <v>31</v>
       </c>
@@ -5485,7 +5650,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="29" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -5527,7 +5692,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="30" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -5569,7 +5734,7 @@
         <v>0.32999999999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -5611,7 +5776,7 @@
         <v>68000</v>
       </c>
     </row>
-    <row r="32" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>164</v>
       </c>
@@ -5641,7 +5806,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="33" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -5683,7 +5848,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>165</v>
       </c>
@@ -5713,7 +5878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -5753,7 +5918,7 @@
         <v>404655.3105184834</v>
       </c>
     </row>
-    <row r="36" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>166</v>
       </c>
@@ -5783,7 +5948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -5817,7 +5982,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>167</v>
       </c>
@@ -5834,7 +5999,7 @@
       <c r="N38" s="130"/>
       <c r="O38" s="130"/>
     </row>
-    <row r="39" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -5867,7 +6032,7 @@
       <c r="N39" s="136"/>
       <c r="O39" s="136"/>
     </row>
-    <row r="40" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -5897,7 +6062,7 @@
       <c r="N40" s="137"/>
       <c r="O40" s="137"/>
     </row>
-    <row r="41" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>79</v>
       </c>
@@ -5927,7 +6092,7 @@
       <c r="N41" s="137"/>
       <c r="O41" s="137"/>
     </row>
-    <row r="42" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
@@ -5943,7 +6108,7 @@
       <c r="N42" s="130"/>
       <c r="O42" s="130"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
       <c r="F43" s="18"/>
@@ -5955,7 +6120,7 @@
       <c r="N43" s="130"/>
       <c r="O43" s="130"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="39" t="s">
         <v>80</v>
       </c>
@@ -5975,7 +6140,7 @@
       <c r="N44" s="130"/>
       <c r="O44" s="130"/>
     </row>
-    <row r="45" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="J45" s="124" t="s">
         <v>205</v>
       </c>
@@ -5987,7 +6152,7 @@
       <c r="N45" s="130"/>
       <c r="O45" s="130"/>
     </row>
-    <row r="46" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>4</v>
       </c>
@@ -6016,8 +6181,8 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="47" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>0</v>
       </c>
@@ -6045,7 +6210,7 @@
         <v>1049205.8974809602</v>
       </c>
     </row>
-    <row r="49" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>5</v>
       </c>
@@ -6073,7 +6238,7 @@
         <v>304269.71026947844</v>
       </c>
     </row>
-    <row r="50" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>14</v>
       </c>
@@ -6102,7 +6267,7 @@
         <v>744936.18721148185</v>
       </c>
     </row>
-    <row r="51" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>43</v>
       </c>
@@ -6130,7 +6295,7 @@
         <v>125904.70769771522</v>
       </c>
     </row>
-    <row r="52" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>44</v>
       </c>
@@ -6158,7 +6323,7 @@
         <v>367222.06411833607</v>
       </c>
     </row>
-    <row r="53" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>45</v>
       </c>
@@ -6187,7 +6352,7 @@
       </c>
       <c r="J53" s="116"/>
     </row>
-    <row r="54" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>15</v>
       </c>
@@ -6216,7 +6381,7 @@
         <v>188857.06154657292</v>
       </c>
     </row>
-    <row r="55" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>168</v>
       </c>
@@ -6242,7 +6407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>169</v>
       </c>
@@ -6268,7 +6433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>13</v>
       </c>
@@ -6298,7 +6463,7 @@
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
     </row>
-    <row r="58" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>46</v>
       </c>
@@ -6325,7 +6490,7 @@
       </c>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>6</v>
       </c>
@@ -6354,7 +6519,7 @@
         <v>180097.67265782671</v>
       </c>
     </row>
-    <row r="60" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
         <v>7</v>
       </c>
@@ -6383,7 +6548,7 @@
       </c>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:10" ht="16.8" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>8</v>
       </c>
@@ -6413,7 +6578,7 @@
       </c>
       <c r="I61" s="79"/>
     </row>
-    <row r="62" spans="1:10" ht="16.8" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>3</v>
       </c>
@@ -6442,7 +6607,7 @@
       </c>
       <c r="I62" s="79"/>
     </row>
-    <row r="63" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>47</v>
       </c>
@@ -6472,7 +6637,7 @@
       </c>
       <c r="I63" s="79"/>
     </row>
-    <row r="64" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
       <c r="B64" s="25"/>
       <c r="C64" s="1"/>
@@ -6482,7 +6647,7 @@
       <c r="G64" s="1"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="4"/>
       <c r="B65" s="25"/>
       <c r="C65" s="1"/>
@@ -6491,7 +6656,7 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="39" t="s">
         <v>81</v>
       </c>
@@ -6503,10 +6668,10 @@
       <c r="G66" s="39"/>
       <c r="H66" s="39"/>
     </row>
-    <row r="67" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A67" s="8"/>
     </row>
-    <row r="68" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>9</v>
       </c>
@@ -6535,10 +6700,10 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="69" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
     </row>
-    <row r="70" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>61</v>
       </c>
@@ -6564,7 +6729,7 @@
         <v>1128.0864237167407</v>
       </c>
     </row>
-    <row r="71" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>48</v>
       </c>
@@ -6592,7 +6757,7 @@
         <v>146888.82564733445</v>
       </c>
     </row>
-    <row r="72" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>49</v>
       </c>
@@ -6620,7 +6785,7 @@
         <v>146888.82564733445</v>
       </c>
     </row>
-    <row r="73" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>50</v>
       </c>
@@ -6648,7 +6813,7 @@
         <v>125904.70769771522</v>
       </c>
     </row>
-    <row r="74" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>170</v>
       </c>
@@ -6674,7 +6839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>51</v>
       </c>
@@ -6702,7 +6867,7 @@
         <v>20984.117949619205</v>
       </c>
     </row>
-    <row r="76" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>171</v>
       </c>
@@ -6728,7 +6893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>52</v>
       </c>
@@ -6756,7 +6921,7 @@
         <v>453150.4581090695</v>
       </c>
     </row>
-    <row r="78" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>172</v>
       </c>
@@ -6782,7 +6947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>30</v>
       </c>
@@ -6810,7 +6975,7 @@
         <v>34000</v>
       </c>
     </row>
-    <row r="80" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>173</v>
       </c>
@@ -6836,7 +7001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="16.8" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>10</v>
       </c>
@@ -6865,7 +7030,7 @@
         <v>928945.0214747896</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="16.8" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A82" s="8"/>
       <c r="B82" s="120"/>
       <c r="C82" s="1"/>
@@ -6874,7 +7039,7 @@
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
     </row>
-    <row r="83" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>53</v>
       </c>
@@ -6900,7 +7065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>54</v>
       </c>
@@ -6928,7 +7093,7 @@
         <v>167872.94359695364</v>
       </c>
     </row>
-    <row r="85" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>55</v>
       </c>
@@ -6956,7 +7121,7 @@
         <v>73444.412823667226</v>
       </c>
     </row>
-    <row r="86" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>56</v>
       </c>
@@ -6984,7 +7149,7 @@
         <v>20984.117949619205</v>
       </c>
     </row>
-    <row r="87" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>57</v>
       </c>
@@ -7012,7 +7177,7 @@
         <v>20984.117949619205</v>
       </c>
     </row>
-    <row r="88" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>174</v>
       </c>
@@ -7038,7 +7203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
         <v>58</v>
       </c>
@@ -7066,7 +7231,7 @@
         <v>31476.176924428804</v>
       </c>
     </row>
-    <row r="90" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>175</v>
       </c>
@@ -7092,7 +7257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
         <v>36</v>
       </c>
@@ -7120,7 +7285,7 @@
         <v>165000</v>
       </c>
     </row>
-    <row r="92" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>166</v>
       </c>
@@ -7146,7 +7311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>37</v>
       </c>
@@ -7174,7 +7339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>167</v>
       </c>
@@ -7200,7 +7365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>11</v>
       </c>
@@ -7228,7 +7393,7 @@
         <v>449183.25223050162</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="16.8" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>12</v>
       </c>
@@ -7257,8 +7422,8 @@
         <v>928945.0214747896</v>
       </c>
     </row>
-    <row r="97" spans="1:19" ht="16.8" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="98" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:19" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="98" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>59</v>
       </c>
@@ -7286,7 +7451,7 @@
         <v>944063.45439389488</v>
       </c>
     </row>
-    <row r="99" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>52</v>
       </c>
@@ -7315,7 +7480,7 @@
         <v>453150.4581090695</v>
       </c>
     </row>
-    <row r="100" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A100" s="14" t="s">
         <v>60</v>
       </c>
@@ -7344,8 +7509,8 @@
         <v>490912.99628482538</v>
       </c>
     </row>
-    <row r="101" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3"/>
-    <row r="102" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="102" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>40</v>
       </c>
@@ -7370,7 +7535,7 @@
         <v>927816.93505107285</v>
       </c>
     </row>
-    <row r="103" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>41</v>
       </c>
@@ -7395,7 +7560,7 @@
         <v>928945.0214747896</v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="16.8" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:19" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>42</v>
       </c>
@@ -7421,8 +7586,8 @@
         <v>-1128.0864237167407</v>
       </c>
     </row>
-    <row r="105" spans="1:19" ht="16.8" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:19" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A107" s="39" t="s">
         <v>82</v>
       </c>
@@ -7434,10 +7599,10 @@
       <c r="G107" s="39"/>
       <c r="H107" s="39"/>
     </row>
-    <row r="108" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="C108" s="13"/>
     </row>
-    <row r="109" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A109" s="37"/>
       <c r="C109" s="41">
         <f>$C$3</f>
@@ -7470,17 +7635,17 @@
       <c r="R109" s="41"/>
       <c r="S109" s="41"/>
     </row>
-    <row r="110" spans="1:19" ht="3" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3"/>
-    <row r="111" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:19" ht="3" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="111" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A111" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C111" s="30">
-        <f t="shared" ref="C111:G112" si="22">C48</f>
+        <f>C48</f>
         <v>793092</v>
       </c>
       <c r="D111" s="30">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="C111:G112" si="22">D48</f>
         <v>856539.3600000001</v>
       </c>
       <c r="E111" s="30">
@@ -7506,7 +7671,7 @@
       <c r="R111" s="13"/>
       <c r="S111" s="13"/>
     </row>
-    <row r="112" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A112" s="13" t="s">
         <v>5</v>
       </c>
@@ -7541,7 +7706,7 @@
       <c r="R112" s="13"/>
       <c r="S112" s="13"/>
     </row>
-    <row r="113" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A113" s="21" t="s">
         <v>14</v>
       </c>
@@ -7576,7 +7741,7 @@
       <c r="R113" s="115"/>
       <c r="S113" s="115"/>
     </row>
-    <row r="114" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A114" s="13" t="s">
         <v>43</v>
       </c>
@@ -7611,7 +7776,7 @@
       <c r="R114" s="13"/>
       <c r="S114" s="13"/>
     </row>
-    <row r="115" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A115" s="13" t="s">
         <v>44</v>
       </c>
@@ -7646,7 +7811,7 @@
       <c r="R115" s="13"/>
       <c r="S115" s="13"/>
     </row>
-    <row r="116" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A116" s="13" t="s">
         <v>45</v>
       </c>
@@ -7681,7 +7846,7 @@
       <c r="R116" s="13"/>
       <c r="S116" s="13"/>
     </row>
-    <row r="117" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A117" s="21" t="s">
         <v>15</v>
       </c>
@@ -7716,7 +7881,7 @@
       <c r="R117" s="115"/>
       <c r="S117" s="115"/>
     </row>
-    <row r="118" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A118" s="13" t="s">
         <v>62</v>
       </c>
@@ -7751,7 +7916,7 @@
       <c r="R118" s="13"/>
       <c r="S118" s="13"/>
     </row>
-    <row r="119" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A119" s="21" t="s">
         <v>63</v>
       </c>
@@ -7786,7 +7951,7 @@
       <c r="R119" s="115"/>
       <c r="S119" s="115"/>
     </row>
-    <row r="120" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A120" s="13" t="s">
         <v>60</v>
       </c>
@@ -7821,7 +7986,7 @@
       <c r="R120" s="13"/>
       <c r="S120" s="13"/>
     </row>
-    <row r="121" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A121" s="21" t="s">
         <v>64</v>
       </c>
@@ -7856,7 +8021,7 @@
       <c r="R121" s="115"/>
       <c r="S121" s="115"/>
     </row>
-    <row r="122" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A122" s="13" t="s">
         <v>49</v>
       </c>
@@ -7891,7 +8056,7 @@
       <c r="R122" s="13"/>
       <c r="S122" s="13"/>
     </row>
-    <row r="123" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A123" s="13" t="s">
         <v>50</v>
       </c>
@@ -7926,7 +8091,7 @@
       <c r="R123" s="13"/>
       <c r="S123" s="13"/>
     </row>
-    <row r="124" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A124" s="13" t="s">
         <v>184</v>
       </c>
@@ -7961,7 +8126,7 @@
       <c r="R124" s="13"/>
       <c r="S124" s="13"/>
     </row>
-    <row r="125" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A125" s="13" t="s">
         <v>54</v>
       </c>
@@ -7996,7 +8161,7 @@
       <c r="R125" s="13"/>
       <c r="S125" s="13"/>
     </row>
-    <row r="126" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A126" s="13" t="s">
         <v>55</v>
       </c>
@@ -8031,7 +8196,7 @@
       <c r="R126" s="13"/>
       <c r="S126" s="13"/>
     </row>
-    <row r="127" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A127" s="13" t="s">
         <v>56</v>
       </c>
@@ -8066,7 +8231,7 @@
       <c r="R127" s="13"/>
       <c r="S127" s="13"/>
     </row>
-    <row r="128" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A128" s="13" t="s">
         <v>57</v>
       </c>
@@ -8101,7 +8266,7 @@
       <c r="R128" s="13"/>
       <c r="S128" s="13"/>
     </row>
-    <row r="129" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A129" s="13" t="s">
         <v>185</v>
       </c>
@@ -8136,7 +8301,7 @@
       <c r="R129" s="13"/>
       <c r="S129" s="13"/>
     </row>
-    <row r="130" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A130" s="21" t="s">
         <v>65</v>
       </c>
@@ -8171,7 +8336,7 @@
       <c r="R130" s="115"/>
       <c r="S130" s="115"/>
     </row>
-    <row r="131" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A131" s="21" t="s">
         <v>66</v>
       </c>
@@ -8206,7 +8371,7 @@
       <c r="R131" s="115"/>
       <c r="S131" s="115"/>
     </row>
-    <row r="132" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A132" s="13" t="s">
         <v>59</v>
       </c>
@@ -8241,7 +8406,7 @@
       <c r="R132" s="13"/>
       <c r="S132" s="13"/>
     </row>
-    <row r="133" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A133" s="13" t="s">
         <v>186</v>
       </c>
@@ -8276,7 +8441,7 @@
       <c r="R133" s="13"/>
       <c r="S133" s="13"/>
     </row>
-    <row r="134" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A134" s="13" t="s">
         <v>187</v>
       </c>
@@ -8311,7 +8476,7 @@
       <c r="R134" s="13"/>
       <c r="S134" s="13"/>
     </row>
-    <row r="135" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A135" s="21" t="s">
         <v>67</v>
       </c>
@@ -8324,7 +8489,7 @@
         <v>-44867.200795200071</v>
       </c>
       <c r="E135" s="31">
-        <f t="shared" ref="D135:G135" si="31">SUM(E132:E134)</f>
+        <f t="shared" ref="E135:G135" si="31">SUM(E132:E134)</f>
         <v>-47559.23284291185</v>
       </c>
       <c r="F135" s="31">
@@ -8346,7 +8511,7 @@
       <c r="R135" s="115"/>
       <c r="S135" s="115"/>
     </row>
-    <row r="136" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A136" s="21" t="s">
         <v>68</v>
       </c>
@@ -8381,7 +8546,7 @@
       <c r="R136" s="115"/>
       <c r="S136" s="115"/>
     </row>
-    <row r="137" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A137" s="21" t="s">
         <v>69</v>
       </c>
@@ -8416,7 +8581,7 @@
       <c r="R137" s="115"/>
       <c r="S137" s="115"/>
     </row>
-    <row r="138" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A138" s="13" t="s">
         <v>168</v>
       </c>
@@ -8451,7 +8616,7 @@
       <c r="R138" s="13"/>
       <c r="S138" s="13"/>
     </row>
-    <row r="139" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A139" s="13" t="s">
         <v>169</v>
       </c>
@@ -8486,7 +8651,7 @@
       <c r="R139" s="13"/>
       <c r="S139" s="13"/>
     </row>
-    <row r="140" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A140" s="13" t="s">
         <v>188</v>
       </c>
@@ -8521,7 +8686,7 @@
       <c r="R140" s="13"/>
       <c r="S140" s="13"/>
     </row>
-    <row r="141" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A141" s="21" t="s">
         <v>76</v>
       </c>
@@ -8556,7 +8721,7 @@
       <c r="R141" s="115"/>
       <c r="S141" s="115"/>
     </row>
-    <row r="142" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A142" s="13" t="s">
         <v>51</v>
       </c>
@@ -8591,7 +8756,7 @@
       <c r="R142" s="13"/>
       <c r="S142" s="13"/>
     </row>
-    <row r="143" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A143" s="13" t="s">
         <v>189</v>
       </c>
@@ -8626,7 +8791,7 @@
       <c r="R143" s="13"/>
       <c r="S143" s="13"/>
     </row>
-    <row r="144" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A144" s="13" t="s">
         <v>58</v>
       </c>
@@ -8661,7 +8826,7 @@
       <c r="R144" s="13"/>
       <c r="S144" s="13"/>
     </row>
-    <row r="145" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A145" s="13" t="s">
         <v>190</v>
       </c>
@@ -8696,7 +8861,7 @@
       <c r="R145" s="13"/>
       <c r="S145" s="13"/>
     </row>
-    <row r="146" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A146" s="13" t="s">
         <v>30</v>
       </c>
@@ -8731,7 +8896,7 @@
       <c r="R146" s="13"/>
       <c r="S146" s="13"/>
     </row>
-    <row r="147" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A147" s="13" t="s">
         <v>191</v>
       </c>
@@ -8766,7 +8931,7 @@
       <c r="R147" s="13"/>
       <c r="S147" s="13"/>
     </row>
-    <row r="148" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A148" s="13" t="s">
         <v>37</v>
       </c>
@@ -8801,7 +8966,7 @@
       <c r="R148" s="13"/>
       <c r="S148" s="13"/>
     </row>
-    <row r="149" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A149" s="13" t="s">
         <v>192</v>
       </c>
@@ -8836,7 +9001,7 @@
       <c r="R149" s="13"/>
       <c r="S149" s="13"/>
     </row>
-    <row r="150" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A150" s="21" t="s">
         <v>77</v>
       </c>
@@ -8871,7 +9036,7 @@
       <c r="R150" s="115"/>
       <c r="S150" s="115"/>
     </row>
-    <row r="151" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A151" s="21" t="s">
         <v>72</v>
       </c>
@@ -8906,7 +9071,7 @@
       <c r="R151" s="115"/>
       <c r="S151" s="115"/>
     </row>
-    <row r="152" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A152" s="21" t="s">
         <v>73</v>
       </c>
@@ -8941,7 +9106,7 @@
       <c r="R152" s="115"/>
       <c r="S152" s="115"/>
     </row>
-    <row r="153" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A153" s="13" t="s">
         <v>188</v>
       </c>
@@ -8976,7 +9141,7 @@
       <c r="R153" s="13"/>
       <c r="S153" s="13"/>
     </row>
-    <row r="154" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A154" s="13" t="s">
         <v>193</v>
       </c>
@@ -9011,7 +9176,7 @@
       <c r="R154" s="13"/>
       <c r="S154" s="13"/>
     </row>
-    <row r="155" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A155" s="13" t="s">
         <v>53</v>
       </c>
@@ -9046,7 +9211,7 @@
       <c r="R155" s="13"/>
       <c r="S155" s="13"/>
     </row>
-    <row r="156" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A156" s="13" t="s">
         <v>36</v>
       </c>
@@ -9081,7 +9246,7 @@
       <c r="R156" s="13"/>
       <c r="S156" s="13"/>
     </row>
-    <row r="157" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A157" s="21" t="s">
         <v>70</v>
       </c>
@@ -9116,7 +9281,7 @@
       <c r="R157" s="13"/>
       <c r="S157" s="13"/>
     </row>
-    <row r="158" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A158" s="21" t="s">
         <v>71</v>
       </c>
@@ -9151,13 +9316,13 @@
       <c r="R158" s="115"/>
       <c r="S158" s="115"/>
     </row>
-    <row r="159" spans="1:19" ht="3.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:19" ht="3.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="D159" s="32"/>
       <c r="E159" s="32"/>
       <c r="F159" s="32"/>
       <c r="G159" s="32"/>
     </row>
-    <row r="160" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A160" s="13" t="s">
         <v>3</v>
       </c>
@@ -9192,7 +9357,7 @@
       <c r="R160" s="13"/>
       <c r="S160" s="13"/>
     </row>
-    <row r="161" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A161" s="21" t="s">
         <v>74</v>
       </c>
@@ -9227,13 +9392,13 @@
       <c r="R161" s="115"/>
       <c r="S161" s="115"/>
     </row>
-    <row r="162" spans="1:19" ht="3.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:19" ht="3.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="D162" s="32"/>
       <c r="E162" s="32"/>
       <c r="F162" s="32"/>
       <c r="G162" s="32"/>
     </row>
-    <row r="163" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A163" s="20" t="s">
         <v>78</v>
       </c>
@@ -9268,7 +9433,7 @@
       <c r="R163" s="115"/>
       <c r="S163" s="115"/>
     </row>
-    <row r="164" spans="1:19" ht="3" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:19" ht="3" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A164" s="23"/>
       <c r="C164" s="24"/>
       <c r="D164" s="24"/>
@@ -9276,7 +9441,7 @@
       <c r="F164" s="24"/>
       <c r="G164" s="24"/>
     </row>
-    <row r="165" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A165" s="35" t="s">
         <v>75</v>
       </c>
@@ -9301,7 +9466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A166" s="35" t="s">
         <v>75</v>
       </c>
@@ -9326,8 +9491,8 @@
         <v>-1.6007106751203537E-10</v>
       </c>
     </row>
-    <row r="167" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3"/>
-    <row r="169" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="169" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A169" s="39" t="s">
         <v>84</v>
       </c>
@@ -9339,8 +9504,8 @@
       <c r="G169" s="39"/>
       <c r="H169" s="39"/>
     </row>
-    <row r="170" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3"/>
-    <row r="171" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="171" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A171" s="68" t="s">
         <v>94</v>
       </c>
@@ -9352,8 +9517,8 @@
       <c r="G171" s="69"/>
       <c r="H171" s="69"/>
     </row>
-    <row r="172" spans="1:19" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="173" spans="1:19" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:19" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="173" spans="1:19" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A173" s="75" t="s">
         <v>147</v>
       </c>
@@ -9365,7 +9530,7 @@
       <c r="G173" s="76"/>
       <c r="H173" s="76"/>
     </row>
-    <row r="174" spans="1:19" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:19" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>85</v>
       </c>
@@ -9374,7 +9539,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="175" spans="1:19" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:19" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>86</v>
       </c>
@@ -9383,8 +9548,8 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:19" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="177" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:19" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="177" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B177" s="28">
         <f>$B$3</f>
         <v>2022</v>
@@ -9413,7 +9578,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="178" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B178" s="74">
         <f>DATE(B177,12,31)</f>
         <v>44926</v>
@@ -9443,7 +9608,7 @@
         <v>46752</v>
       </c>
     </row>
-    <row r="179" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B179" s="28"/>
       <c r="C179" s="41"/>
       <c r="D179" s="41"/>
@@ -9452,7 +9617,7 @@
       <c r="G179" s="41"/>
       <c r="H179" s="65"/>
     </row>
-    <row r="180" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>131</v>
       </c>
@@ -9484,7 +9649,7 @@
         <v>2106741.4065030455</v>
       </c>
     </row>
-    <row r="181" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>134</v>
       </c>
@@ -9499,7 +9664,7 @@
       </c>
       <c r="H181" s="13"/>
     </row>
-    <row r="182" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A182" s="20" t="s">
         <v>132</v>
       </c>
@@ -9526,7 +9691,7 @@
       </c>
       <c r="H182" s="13"/>
     </row>
-    <row r="183" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B183" s="27"/>
       <c r="C183" s="13"/>
       <c r="D183" s="13"/>
@@ -9535,7 +9700,7 @@
       <c r="G183" s="13"/>
       <c r="H183" s="13"/>
     </row>
-    <row r="184" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>133</v>
       </c>
@@ -9567,7 +9732,7 @@
         <v>11282.086280923648</v>
       </c>
     </row>
-    <row r="185" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>135</v>
       </c>
@@ -9576,7 +9741,7 @@
         <v>11282.086280923648</v>
       </c>
     </row>
-    <row r="186" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A186" s="20" t="s">
         <v>136</v>
       </c>
@@ -9603,7 +9768,7 @@
       </c>
       <c r="H186" s="13"/>
     </row>
-    <row r="187" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B187" s="27"/>
       <c r="C187" s="13"/>
       <c r="D187" s="13"/>
@@ -9612,7 +9777,7 @@
       <c r="G187" s="13"/>
       <c r="H187" s="13"/>
     </row>
-    <row r="188" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>88</v>
       </c>
@@ -9625,7 +9790,7 @@
         <v>0.99519984705678166</v>
       </c>
     </row>
-    <row r="189" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>89</v>
       </c>
@@ -9638,7 +9803,7 @@
         <v>4.8001529432183023E-3</v>
       </c>
     </row>
-    <row r="190" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A190" s="20" t="s">
         <v>90</v>
       </c>
@@ -9651,7 +9816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>91</v>
       </c>
@@ -9660,7 +9825,7 @@
         <v>89784</v>
       </c>
     </row>
-    <row r="192" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>92</v>
       </c>
@@ -9669,7 +9834,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="193" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A193" s="14" t="s">
         <v>93</v>
       </c>
@@ -9678,10 +9843,10 @@
         <v>1568885.0732881178</v>
       </c>
     </row>
-    <row r="194" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B194" s="13"/>
     </row>
-    <row r="195" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A195" s="75" t="s">
         <v>145</v>
       </c>
@@ -9693,7 +9858,7 @@
       <c r="G195" s="76"/>
       <c r="H195" s="76"/>
     </row>
-    <row r="196" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="C196" s="147" t="s">
         <v>157</v>
       </c>
@@ -9702,7 +9867,7 @@
       <c r="F196" s="147"/>
       <c r="G196" s="147"/>
     </row>
-    <row r="197" spans="1:8" ht="20.25" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:8" ht="20.25" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="C197" s="148" t="s">
         <v>95</v>
       </c>
@@ -9711,7 +9876,7 @@
       <c r="F197" s="148"/>
       <c r="G197" s="148"/>
     </row>
-    <row r="198" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B198" s="30">
         <f ca="1">B190</f>
         <v>1629101.0732881178</v>
@@ -9736,7 +9901,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="199" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A199" s="146" t="s">
         <v>96</v>
       </c>
@@ -9760,7 +9925,7 @@
         <v>3387501.2610190972</v>
       </c>
     </row>
-    <row r="200" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A200" s="146"/>
       <c r="B200" s="87">
         <f>B199+0.01</f>
@@ -9782,7 +9947,7 @@
         <v>2425267.1030343277</v>
       </c>
     </row>
-    <row r="201" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A201" s="146"/>
       <c r="B201" s="87">
         <f t="shared" ref="B201:B203" si="52">B200+0.01</f>
@@ -9804,7 +9969,7 @@
         <v>1873693.7785326121</v>
       </c>
     </row>
-    <row r="202" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A202" s="146"/>
       <c r="B202" s="87">
         <f t="shared" si="52"/>
@@ -9826,7 +9991,7 @@
         <v>1516600.5946441719</v>
       </c>
     </row>
-    <row r="203" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A203" s="146"/>
       <c r="B203" s="87">
         <f t="shared" si="52"/>
@@ -9848,7 +10013,7 @@
         <v>1266871.9557497974</v>
       </c>
     </row>
-    <row r="204" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A204" s="114"/>
       <c r="B204" s="42"/>
       <c r="C204" s="13"/>
@@ -9857,7 +10022,7 @@
       <c r="F204" s="13"/>
       <c r="G204" s="13"/>
     </row>
-    <row r="205" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A205" s="114"/>
       <c r="B205" s="42"/>
       <c r="C205" s="13"/>
@@ -9866,7 +10031,7 @@
       <c r="F205" s="13"/>
       <c r="G205" s="13"/>
     </row>
-    <row r="206" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A206" s="75" t="s">
         <v>146</v>
       </c>
@@ -9878,11 +10043,11 @@
       <c r="G206" s="76"/>
       <c r="H206" s="76"/>
     </row>
-    <row r="207" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A207" s="2"/>
       <c r="B207" s="42"/>
     </row>
-    <row r="208" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>144</v>
       </c>
@@ -9915,7 +10080,7 @@
         <v>2106741.4065030455</v>
       </c>
     </row>
-    <row r="209" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>98</v>
       </c>
@@ -9948,7 +10113,7 @@
         <v>11282.086280923648</v>
       </c>
     </row>
-    <row r="210" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A210" s="20" t="s">
         <v>97</v>
       </c>
@@ -9981,27 +10146,27 @@
         <v>2118023.4927839693</v>
       </c>
     </row>
-    <row r="211" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="212" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="213" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="214" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="215" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="216" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="217" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="218" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="219" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="220" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="221" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="222" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="223" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="224" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="225" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="226" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="227" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="228" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="229" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="230" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3"/>
-    <row r="231" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="212" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="213" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="214" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="215" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="216" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="217" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="218" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="219" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="220" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="221" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="222" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="223" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="224" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="225" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="226" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="227" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="228" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="229" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="230" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="231" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A231" s="68" t="s">
         <v>99</v>
       </c>
@@ -10013,13 +10178,13 @@
       <c r="G231" s="69"/>
       <c r="H231" s="69"/>
     </row>
-    <row r="232" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="233" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="233" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="234" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>101</v>
       </c>
@@ -10039,7 +10204,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="235" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>105</v>
       </c>
@@ -10059,7 +10224,7 @@
         <v>3.65</v>
       </c>
     </row>
-    <row r="236" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>106</v>
       </c>
@@ -10079,7 +10244,7 @@
         <v>3.34</v>
       </c>
     </row>
-    <row r="237" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A237" s="14" t="s">
         <v>107</v>
       </c>
@@ -10104,13 +10269,13 @@
         <v>3.4950000000000001</v>
       </c>
     </row>
-    <row r="238" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="239" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="240" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="240" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>176</v>
       </c>
@@ -10127,7 +10292,7 @@
         <v>4.5599999999999996</v>
       </c>
     </row>
-    <row r="241" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>177</v>
       </c>
@@ -10144,7 +10309,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="242" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>178</v>
       </c>
@@ -10161,7 +10326,7 @@
         <v>2.34</v>
       </c>
     </row>
-    <row r="243" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>180</v>
       </c>
@@ -10178,7 +10343,7 @@
         <v>4.32</v>
       </c>
     </row>
-    <row r="244" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>181</v>
       </c>
@@ -10195,7 +10360,7 @@
         <v>1.99</v>
       </c>
     </row>
-    <row r="245" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A245" s="14" t="s">
         <v>115</v>
       </c>
@@ -10217,13 +10382,13 @@
         <v>3.0620000000000003</v>
       </c>
     </row>
-    <row r="246" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="247" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="248" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="248" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>112</v>
       </c>
@@ -10231,7 +10396,7 @@
         <v>44892</v>
       </c>
     </row>
-    <row r="249" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>179</v>
       </c>
@@ -10239,10 +10404,10 @@
         <v>20223</v>
       </c>
     </row>
-    <row r="250" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B250" s="27"/>
     </row>
-    <row r="251" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B251" s="28">
         <v>2022</v>
       </c>
@@ -10253,7 +10418,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="252" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>113</v>
       </c>
@@ -10272,7 +10437,7 @@
       <c r="E252" s="13"/>
       <c r="F252" s="13"/>
     </row>
-    <row r="253" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>114</v>
       </c>
@@ -10291,7 +10456,7 @@
       <c r="E253" s="13"/>
       <c r="F253" s="13"/>
     </row>
-    <row r="254" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>182</v>
       </c>
@@ -10311,7 +10476,7 @@
       <c r="F254" s="13"/>
       <c r="H254" s="13"/>
     </row>
-    <row r="255" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>108</v>
       </c>
@@ -10325,7 +10490,7 @@
       </c>
       <c r="D255" s="34"/>
     </row>
-    <row r="256" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>111</v>
       </c>
@@ -10344,7 +10509,7 @@
       <c r="E256" s="13"/>
       <c r="F256" s="13"/>
     </row>
-    <row r="257" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A257" s="70" t="s">
         <v>107</v>
       </c>
@@ -10360,21 +10525,21 @@
       <c r="E257" s="72"/>
       <c r="F257" s="72"/>
     </row>
-    <row r="258" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A258" s="38"/>
       <c r="B258" s="38"/>
       <c r="C258" s="103"/>
       <c r="D258" s="103"/>
       <c r="E258" s="13"/>
     </row>
-    <row r="259" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A259" s="38"/>
       <c r="B259" s="38"/>
       <c r="C259" s="103"/>
       <c r="D259" s="103"/>
       <c r="E259" s="13"/>
     </row>
-    <row r="260" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A260" s="68" t="s">
         <v>156</v>
       </c>
@@ -10386,7 +10551,7 @@
       <c r="G260" s="69"/>
       <c r="H260" s="69"/>
     </row>
-    <row r="261" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A261" s="98"/>
       <c r="B261" s="98"/>
       <c r="C261" s="98"/>
@@ -10396,7 +10561,7 @@
       <c r="G261" s="100"/>
       <c r="H261" s="100"/>
     </row>
-    <row r="262" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A262" s="98"/>
       <c r="B262" s="98"/>
       <c r="C262" s="113" t="s">
@@ -10414,7 +10579,7 @@
       <c r="G262" s="100"/>
       <c r="H262" s="100"/>
     </row>
-    <row r="263" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>152</v>
       </c>
@@ -10438,7 +10603,7 @@
       <c r="G263" s="100"/>
       <c r="H263" s="100"/>
     </row>
-    <row r="264" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>153</v>
       </c>
@@ -10462,7 +10627,7 @@
       <c r="G264" s="98"/>
       <c r="H264" s="98"/>
     </row>
-    <row r="265" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>154</v>
       </c>
@@ -10486,7 +10651,7 @@
       <c r="G265" s="100"/>
       <c r="H265" s="100"/>
     </row>
-    <row r="266" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>155</v>
       </c>
@@ -10510,7 +10675,7 @@
       <c r="G266" s="100"/>
       <c r="H266" s="100"/>
     </row>
-    <row r="267" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A267" s="98"/>
       <c r="B267" s="98"/>
       <c r="C267" s="98"/>
@@ -10520,7 +10685,7 @@
       <c r="G267" s="100"/>
       <c r="H267" s="100"/>
     </row>
-    <row r="268" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A268" s="98"/>
       <c r="B268" s="98"/>
       <c r="C268" s="98"/>
@@ -10530,7 +10695,7 @@
       <c r="G268" s="100"/>
       <c r="H268" s="100"/>
     </row>
-    <row r="269" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A269" s="98"/>
       <c r="B269" s="97"/>
       <c r="C269" s="98"/>
@@ -10540,7 +10705,7 @@
       <c r="G269" s="100"/>
       <c r="H269" s="100"/>
     </row>
-    <row r="270" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A270" s="98"/>
       <c r="B270" s="98"/>
       <c r="C270" s="98"/>
@@ -10550,7 +10715,7 @@
       <c r="G270" s="100"/>
       <c r="H270" s="100"/>
     </row>
-    <row r="271" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A271" s="98"/>
       <c r="B271" s="98"/>
       <c r="C271" s="98"/>
@@ -10560,7 +10725,7 @@
       <c r="G271" s="100"/>
       <c r="H271" s="100"/>
     </row>
-    <row r="272" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A272" s="98"/>
       <c r="B272" s="98"/>
       <c r="C272" s="98"/>
@@ -10570,7 +10735,7 @@
       <c r="G272" s="100"/>
       <c r="H272" s="100"/>
     </row>
-    <row r="273" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A273" s="98"/>
       <c r="B273" s="98"/>
       <c r="C273" s="98"/>
@@ -10580,7 +10745,7 @@
       <c r="G273" s="100"/>
       <c r="H273" s="100"/>
     </row>
-    <row r="274" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A274" s="98"/>
       <c r="B274" s="98"/>
       <c r="C274" s="98"/>
@@ -10590,7 +10755,7 @@
       <c r="G274" s="100"/>
       <c r="H274" s="100"/>
     </row>
-    <row r="275" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A275" s="98"/>
       <c r="B275" s="98"/>
       <c r="C275" s="98"/>
@@ -10600,10 +10765,10 @@
       <c r="G275" s="98"/>
       <c r="H275" s="100"/>
     </row>
-    <row r="276" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A276" s="98"/>
     </row>
-    <row r="277" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A277" s="98"/>
       <c r="B277" s="98"/>
       <c r="C277" s="98"/>
@@ -10613,7 +10778,7 @@
       <c r="G277" s="98"/>
       <c r="H277" s="98"/>
     </row>
-    <row r="278" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A278" s="98"/>
       <c r="B278" s="98"/>
       <c r="C278" s="98"/>
@@ -10623,7 +10788,7 @@
       <c r="G278" s="98"/>
       <c r="H278" s="98"/>
     </row>
-    <row r="279" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A279" s="98"/>
       <c r="B279" s="98"/>
       <c r="C279" s="98"/>
@@ -10633,7 +10798,7 @@
       <c r="G279" s="98"/>
       <c r="H279" s="98"/>
     </row>
-    <row r="280" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A280" s="98"/>
       <c r="B280" s="98"/>
       <c r="C280" s="98"/>
@@ -10643,7 +10808,7 @@
       <c r="G280" s="98"/>
       <c r="H280" s="98"/>
     </row>
-    <row r="281" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A281" s="98"/>
       <c r="B281" s="98"/>
       <c r="C281" s="98"/>
@@ -10653,7 +10818,7 @@
       <c r="G281" s="98"/>
       <c r="H281" s="98"/>
     </row>
-    <row r="282" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A282" s="98"/>
       <c r="B282" s="98"/>
       <c r="C282" s="98"/>
@@ -10663,7 +10828,7 @@
       <c r="G282" s="98"/>
       <c r="H282" s="98"/>
     </row>
-    <row r="283" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A283" s="98"/>
       <c r="B283" s="98"/>
       <c r="C283" s="98"/>
@@ -10673,7 +10838,7 @@
       <c r="G283" s="98"/>
       <c r="H283" s="98"/>
     </row>
-    <row r="284" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A284" s="98"/>
       <c r="B284" s="98"/>
       <c r="C284" s="98"/>
@@ -10683,7 +10848,7 @@
       <c r="G284" s="98"/>
       <c r="H284" s="98"/>
     </row>
-    <row r="285" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A285" s="98"/>
       <c r="B285" s="98"/>
       <c r="C285" s="98"/>
@@ -10693,7 +10858,7 @@
       <c r="G285" s="98"/>
       <c r="H285" s="98"/>
     </row>
-    <row r="286" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A286" s="98"/>
       <c r="B286" s="98"/>
       <c r="C286" s="98"/>
@@ -10703,7 +10868,7 @@
       <c r="G286" s="98"/>
       <c r="H286" s="98"/>
     </row>
-    <row r="287" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:8" ht="16.5" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A287" s="98"/>
       <c r="B287" s="98"/>
       <c r="C287" s="98"/>
@@ -10713,15 +10878,15 @@
       <c r="G287" s="98"/>
       <c r="H287" s="98"/>
     </row>
-    <row r="288" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A288" s="38"/>
       <c r="B288" s="38"/>
       <c r="C288" s="103"/>
       <c r="D288" s="103"/>
       <c r="E288" s="13"/>
     </row>
-    <row r="289" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3"/>
-    <row r="290" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="290" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A290" s="68" t="s">
         <v>116</v>
       </c>
@@ -10733,8 +10898,8 @@
       <c r="G290" s="69"/>
       <c r="H290" s="69"/>
     </row>
-    <row r="291" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="292" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="292" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B292" s="28">
         <f>$B$3</f>
         <v>2022</v>
@@ -10763,7 +10928,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="293" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B293" s="46"/>
       <c r="C293" s="43"/>
       <c r="D293" s="43"/>
@@ -10772,7 +10937,7 @@
       <c r="G293" s="43"/>
       <c r="H293" s="44"/>
     </row>
-    <row r="294" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A294" s="50" t="s">
         <v>63</v>
       </c>
@@ -10797,7 +10962,7 @@
         <v>141642.79615992968</v>
       </c>
     </row>
-    <row r="295" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A295" s="50" t="s">
         <v>117</v>
       </c>
@@ -10826,7 +10991,7 @@
         <v>442658.39913425985</v>
       </c>
     </row>
-    <row r="296" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A296" s="50" t="s">
         <v>118</v>
       </c>
@@ -10851,10 +11016,10 @@
         <v>442658.39913425985</v>
       </c>
     </row>
-    <row r="297" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A297" s="51"/>
     </row>
-    <row r="298" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A298" s="50" t="s">
         <v>119</v>
       </c>
@@ -10879,7 +11044,7 @@
         <v>0.33918110268136359</v>
       </c>
     </row>
-    <row r="299" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A299" s="52" t="s">
         <v>120</v>
       </c>
@@ -10904,7 +11069,7 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="300" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A300" s="50" t="s">
         <v>121</v>
       </c>
@@ -10930,7 +11095,7 @@
         <v>0.25218110268136362</v>
       </c>
     </row>
-    <row r="301" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A301" s="61" t="str">
         <f t="shared" ref="A301" si="64">A295</f>
         <v>COEi</v>
@@ -10957,7 +11122,7 @@
       </c>
       <c r="H301" s="55"/>
     </row>
-    <row r="302" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A302" s="50" t="s">
         <v>137</v>
       </c>
@@ -10987,7 +11152,7 @@
         <v>1664083.0073687856</v>
       </c>
     </row>
-    <row r="303" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A303" s="52" t="s">
         <v>138</v>
       </c>
@@ -11002,7 +11167,7 @@
       </c>
       <c r="H303" s="13"/>
     </row>
-    <row r="304" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A304" s="50" t="s">
         <v>139</v>
       </c>
@@ -11029,7 +11194,7 @@
       </c>
       <c r="H304" s="13"/>
     </row>
-    <row r="305" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A305" s="59"/>
       <c r="B305" s="60"/>
       <c r="C305" s="54"/>
@@ -11039,7 +11204,7 @@
       <c r="G305" s="54"/>
       <c r="H305" s="13"/>
     </row>
-    <row r="306" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A306" s="53" t="s">
         <v>130</v>
       </c>
@@ -11048,7 +11213,7 @@
         <v>1294831.1389763735</v>
       </c>
     </row>
-    <row r="307" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A307" s="53" t="s">
         <v>127</v>
       </c>
@@ -11057,7 +11222,7 @@
         <v>326450</v>
       </c>
     </row>
-    <row r="308" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A308" s="73" t="s">
         <v>128</v>
       </c>
@@ -11066,7 +11231,7 @@
         <v>1621281.1389763735</v>
       </c>
     </row>
-    <row r="309" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A309" s="67" t="s">
         <v>75</v>
       </c>
@@ -11075,7 +11240,7 @@
         <v>1621281.1389763737</v>
       </c>
     </row>
-    <row r="310" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A310" s="51"/>
       <c r="B310" s="13"/>
       <c r="C310" s="54"/>
@@ -11084,7 +11249,7 @@
       <c r="F310" s="54"/>
       <c r="G310" s="54"/>
     </row>
-    <row r="311" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A311" s="50" t="s">
         <v>76</v>
       </c>
@@ -11110,7 +11275,7 @@
         <v>30.458333440351996</v>
       </c>
     </row>
-    <row r="312" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A312" s="50" t="s">
         <v>122</v>
       </c>
@@ -11139,7 +11304,7 @@
         <v>23507.941025190401</v>
       </c>
     </row>
-    <row r="313" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A313" s="50" t="s">
         <v>123</v>
       </c>
@@ -11164,10 +11329,10 @@
         <v>23507.941025190401</v>
       </c>
     </row>
-    <row r="314" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A314" s="51"/>
     </row>
-    <row r="315" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A315" s="50" t="s">
         <v>124</v>
       </c>
@@ -11192,7 +11357,7 @@
         <v>1.2637352424971985E-3</v>
       </c>
     </row>
-    <row r="316" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A316" s="52" t="s">
         <v>120</v>
       </c>
@@ -11217,7 +11382,7 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="317" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A317" s="50" t="s">
         <v>121</v>
       </c>
@@ -11243,7 +11408,7 @@
         <v>-8.5736264757502789E-2</v>
       </c>
     </row>
-    <row r="318" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A318" s="61" t="str">
         <f>A312</f>
         <v>CNOEi</v>
@@ -11270,7 +11435,7 @@
       </c>
       <c r="H318" s="55"/>
     </row>
-    <row r="319" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A319" s="50" t="s">
         <v>140</v>
       </c>
@@ -11300,7 +11465,7 @@
         <v>-12225.854744266753</v>
       </c>
     </row>
-    <row r="320" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A320" s="52" t="s">
         <v>141</v>
       </c>
@@ -11315,7 +11480,7 @@
       </c>
       <c r="H320" s="13"/>
     </row>
-    <row r="321" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A321" s="50" t="s">
         <v>142</v>
       </c>
@@ -11342,11 +11507,11 @@
       </c>
       <c r="H321" s="13"/>
     </row>
-    <row r="322" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A322" s="59"/>
       <c r="C322" s="64"/>
     </row>
-    <row r="323" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A323" s="53" t="s">
         <v>143</v>
       </c>
@@ -11355,7 +11520,7 @@
         <v>-18234.065688255952</v>
       </c>
     </row>
-    <row r="324" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A324" s="53" t="s">
         <v>129</v>
       </c>
@@ -11364,7 +11529,7 @@
         <v>26054</v>
       </c>
     </row>
-    <row r="325" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A325" s="73" t="s">
         <v>125</v>
       </c>
@@ -11373,7 +11538,7 @@
         <v>7819.9343117440476</v>
       </c>
     </row>
-    <row r="326" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A326" s="67" t="s">
         <v>75</v>
       </c>
@@ -11382,10 +11547,10 @@
         <v>7819.934311744054</v>
       </c>
     </row>
-    <row r="327" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A327" s="51"/>
     </row>
-    <row r="328" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A328" s="73" t="s">
         <v>126</v>
       </c>
@@ -11394,7 +11559,7 @@
         <v>1629101.0732881175</v>
       </c>
     </row>
-    <row r="329" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A329" s="67" t="s">
         <v>75</v>
       </c>
@@ -11403,51 +11568,51 @@
         <v>1629101.0732881178</v>
       </c>
     </row>
-    <row r="330" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="331" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3"/>
-    <row r="332" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="331" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="332" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="C332" s="13"/>
       <c r="D332" s="13"/>
       <c r="E332" s="13"/>
       <c r="F332" s="13"/>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C333" s="13"/>
       <c r="D333" s="13"/>
       <c r="E333" s="13"/>
       <c r="F333" s="13"/>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C334" s="13"/>
       <c r="D334" s="13"/>
       <c r="E334" s="13"/>
       <c r="F334" s="13"/>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C335" s="13"/>
       <c r="D335" s="13"/>
       <c r="E335" s="13"/>
       <c r="F335" s="13"/>
     </row>
-    <row r="337" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="337" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C337" s="13"/>
       <c r="D337" s="13"/>
       <c r="E337" s="13"/>
       <c r="F337" s="13"/>
     </row>
-    <row r="338" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="338" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C338" s="13"/>
       <c r="D338" s="13"/>
       <c r="E338" s="13"/>
       <c r="F338" s="13"/>
     </row>
-    <row r="339" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="339" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C339" s="13"/>
       <c r="D339" s="13"/>
       <c r="E339" s="13"/>
       <c r="F339" s="13"/>
     </row>
-    <row r="340" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="340" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C340" s="13"/>
       <c r="D340" s="13"/>
       <c r="E340" s="13"/>
@@ -11477,15 +11642,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>11</xdr:col>
-                    <xdr:colOff>22860</xdr:colOff>
+                    <xdr:colOff>19050</xdr:colOff>
                     <xdr:row>43</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>11</xdr:col>
                     <xdr:colOff>1104900</xdr:colOff>
                     <xdr:row>44</xdr:row>
-                    <xdr:rowOff>182880</xdr:rowOff>
+                    <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11499,15 +11664,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>617220</xdr:colOff>
+                    <xdr:colOff>619125</xdr:colOff>
                     <xdr:row>189</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>190</xdr:row>
-                    <xdr:rowOff>198120</xdr:rowOff>
+                    <xdr:rowOff>200025</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11518,4 +11683,484 @@
     </mc:Choice>
   </mc:AlternateContent>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05896313-5679-4DD6-B8EC-08704ECE71D0}">
+  <dimension ref="A1:G40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="70.8984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1" s="153">
+        <v>2022</v>
+      </c>
+      <c r="C1" s="153" t="s">
+        <v>247</v>
+      </c>
+      <c r="D1" s="153" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="116">
+        <f>'MODELO VALORACIÓN SIMPLIFICADO'!B40</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="116">
+        <f>'MODELO VALORACIÓN SIMPLIFICADO'!C40</f>
+        <v>8.6999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G3" s="159" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B4" s="116">
+        <f>('MODELO VALORACIÓN SIMPLIFICADO'!B54+'MODELO VALORACIÓN SIMPLIFICADO'!B100)/'MODELO VALORACIÓN SIMPLIFICADO'!B48</f>
+        <v>0.58106188184977281</v>
+      </c>
+      <c r="G4" s="159" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>208</v>
+      </c>
+      <c r="G5" s="159" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B6" t="e">
+        <f>'MODELO VALORACIÓN SIMPLIFICADO'!B119/'MODELO VALORACIÓN SIMPLIFICADO'!B141</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C6" t="e">
+        <f ca="1">'MODELO VALORACIÓN SIMPLIFICADO'!C119/'MODELO VALORACIÓN SIMPLIFICADO'!C141</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G6" s="159" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7" s="116" t="e">
+        <f>'MODELO VALORACIÓN SIMPLIFICADO'!B119/(-'MODELO VALORACIÓN SIMPLIFICADO'!B136-'MODELO VALORACIÓN SIMPLIFICADO'!B150)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C7" s="116">
+        <f>'MODELO VALORACIÓN SIMPLIFICADO'!C119/(-'MODELO VALORACIÓN SIMPLIFICADO'!C136-'MODELO VALORACIÓN SIMPLIFICADO'!C150)</f>
+        <v>0.71014324570361431</v>
+      </c>
+      <c r="G7" s="159" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="116"/>
+      <c r="C8" s="116"/>
+      <c r="G8" s="159" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B9" s="116">
+        <f>('MODELO VALORACIÓN SIMPLIFICADO'!B96-'MODELO VALORACIÓN SIMPLIFICADO'!B95)/'MODELO VALORACIÓN SIMPLIFICADO'!B96</f>
+        <v>0.52347818148026182</v>
+      </c>
+      <c r="C9" s="116">
+        <f ca="1">('MODELO VALORACIÓN SIMPLIFICADO'!C96-'MODELO VALORACIÓN SIMPLIFICADO'!C95)/'MODELO VALORACIÓN SIMPLIFICADO'!C96</f>
+        <v>0.55957264817289509</v>
+      </c>
+      <c r="E9" s="157" t="s">
+        <v>253</v>
+      </c>
+      <c r="F9" s="158"/>
+      <c r="G9" s="159" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>212</v>
+      </c>
+      <c r="B10" s="116">
+        <f>'MODELO VALORACIÓN SIMPLIFICADO'!B95/'MODELO VALORACIÓN SIMPLIFICADO'!B96</f>
+        <v>0.47652181851973824</v>
+      </c>
+      <c r="C10" s="116">
+        <f ca="1">'MODELO VALORACIÓN SIMPLIFICADO'!C95/'MODELO VALORACIÓN SIMPLIFICADO'!C96</f>
+        <v>0.44042735182710491</v>
+      </c>
+      <c r="E10" s="157"/>
+      <c r="F10" s="158"/>
+      <c r="G10" s="159" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G11" s="159" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>213</v>
+      </c>
+      <c r="B12" s="154">
+        <v>3.4299999999999997E-2</v>
+      </c>
+      <c r="C12" s="154">
+        <v>3.4299999999999997E-2</v>
+      </c>
+      <c r="G12" s="159" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>214</v>
+      </c>
+      <c r="B13" s="154">
+        <v>2.6599999999999999E-2</v>
+      </c>
+      <c r="C13" s="154">
+        <v>2.6599999999999999E-2</v>
+      </c>
+      <c r="G13" s="159" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B14">
+        <v>1.1459577381297801</v>
+      </c>
+      <c r="C14">
+        <v>1.1459577381297801</v>
+      </c>
+      <c r="G14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B15" s="154">
+        <v>3.8399999999999997E-2</v>
+      </c>
+      <c r="C15" s="154">
+        <v>3.8399999999999997E-2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>217</v>
+      </c>
+      <c r="B16" s="154">
+        <f>B12+B14*B13+B15</f>
+        <v>0.10318247583425214</v>
+      </c>
+      <c r="C16" s="154">
+        <f>C12+C14*C13+C15</f>
+        <v>0.10318247583425214</v>
+      </c>
+      <c r="G16" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>218</v>
+      </c>
+      <c r="B17" s="154">
+        <f>(B2-B16*B10)/(B9*(1-'MODELO VALORACIÓN SIMPLIFICADO'!C14))</f>
+        <v>-0.125235913073767</v>
+      </c>
+      <c r="C17" s="154">
+        <f ca="1">(C2-C16*C10)/(C9*(1-'MODELO VALORACIÓN SIMPLIFICADO'!D14))</f>
+        <v>9.9017504516568974E-2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>219</v>
+      </c>
+      <c r="B19" s="151">
+        <f>'MODELO VALORACIÓN SIMPLIFICADO'!B48</f>
+        <v>748200</v>
+      </c>
+      <c r="C19" s="151">
+        <f>'MODELO VALORACIÓN SIMPLIFICADO'!C48</f>
+        <v>793092</v>
+      </c>
+      <c r="D19" s="151">
+        <f>C19-B19</f>
+        <v>44892</v>
+      </c>
+      <c r="G19" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" s="151" t="e">
+        <f>(('MODELO VALORACIÓN SIMPLIFICADO'!B119/'MODELO VALORACIÓN SIMPLIFICADO'!B136)-'MODELO VALORACIÓN SIMPLIFICADO'!$B$40)*'MODELO VALORACIÓN SIMPLIFICADO'!B136</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C20" s="151">
+        <f>(('MODELO VALORACIÓN SIMPLIFICADO'!C119/'MODELO VALORACIÓN SIMPLIFICADO'!C136)-'MODELO VALORACIÓN SIMPLIFICADO'!$C$40)*'MODELO VALORACIÓN SIMPLIFICADO'!C136</f>
+        <v>51586.933613039982</v>
+      </c>
+      <c r="D20" s="151"/>
+      <c r="G20" s="159" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>220</v>
+      </c>
+      <c r="B21" s="151" t="e">
+        <f>(('MODELO VALORACIÓN SIMPLIFICADO'!B141/'MODELO VALORACIÓN SIMPLIFICADO'!B150)-'MODELO VALORACIÓN SIMPLIFICADO'!$B$40)*'MODELO VALORACIÓN SIMPLIFICADO'!B150</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C21" s="151">
+        <f ca="1">(('MODELO VALORACIÓN SIMPLIFICADO'!C141/'MODELO VALORACIÓN SIMPLIFICADO'!C150)-'MODELO VALORACIÓN SIMPLIFICADO'!$C$40)*'MODELO VALORACIÓN SIMPLIFICADO'!C150</f>
+        <v>1828.31196</v>
+      </c>
+      <c r="D21" s="151"/>
+      <c r="G21" s="159" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B22" s="152" t="e">
+        <f>B20+B21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C22" s="152">
+        <f ca="1">C20+C21</f>
+        <v>53415.245573039982</v>
+      </c>
+      <c r="D22" s="152" t="e">
+        <f ca="1">C22-B22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G22" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>222</v>
+      </c>
+      <c r="B23" s="116" t="e">
+        <f>B22/B19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C23" s="116">
+        <f ca="1">C22/C19</f>
+        <v>6.7350629653356711E-2</v>
+      </c>
+      <c r="D23" s="116" t="e">
+        <f ca="1">C23-B23</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>223</v>
+      </c>
+      <c r="C24" s="116">
+        <f>D19/C19</f>
+        <v>5.6603773584905662E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>224</v>
+      </c>
+      <c r="C25" t="e">
+        <f ca="1">C28+C29</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>225</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28" s="154">
+        <f ca="1">C23*C24</f>
+        <v>3.8122997916994364E-3</v>
+      </c>
+      <c r="D28" t="e">
+        <f ca="1">C28/$C$25</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>226</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29" s="154" t="e">
+        <f ca="1">D23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D29" t="e">
+        <f ca="1">C29/$C$25</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B32" s="116">
+        <f>'MODELO VALORACIÓN SIMPLIFICADO'!B61/'MODELO VALORACIÓN SIMPLIFICADO'!B95</f>
+        <v>0.14616747865119334</v>
+      </c>
+      <c r="C32" s="116">
+        <f ca="1">'MODELO VALORACIÓN SIMPLIFICADO'!C61/'MODELO VALORACIÓN SIMPLIFICADO'!C95</f>
+        <v>0.1281874844675461</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>252</v>
+      </c>
+      <c r="B33" s="116">
+        <f>'MODELO VALORACIÓN SIMPLIFICADO'!B61/'MODELO VALORACIÓN SIMPLIFICADO'!B81</f>
+        <v>6.9651992735311669E-2</v>
+      </c>
+      <c r="C33" s="116">
+        <f ca="1">'MODELO VALORACIÓN SIMPLIFICADO'!C61/'MODELO VALORACIÓN SIMPLIFICADO'!C81</f>
+        <v>5.6457274321419483E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>228</v>
+      </c>
+      <c r="B34" s="156">
+        <v>1</v>
+      </c>
+      <c r="C34" s="156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>251</v>
+      </c>
+      <c r="B35" s="116">
+        <f>(B33*B34)/(1-(B33*B34))</f>
+        <v>7.486660066064435E-2</v>
+      </c>
+      <c r="C35" s="116">
+        <f ca="1">(C33*C34)/(1-(C33*C34))</f>
+        <v>5.9835418985204225E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>227</v>
+      </c>
+      <c r="B36" s="116">
+        <f>(B32*B34)/(1-(B32*B34))</f>
+        <v>0.17118987037445152</v>
+      </c>
+      <c r="C36" s="116">
+        <f ca="1">(C32*C34)/(1-(C32*C34))</f>
+        <v>0.14703560935834514</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>230</v>
+      </c>
+      <c r="B38" s="155">
+        <v>0.7</v>
+      </c>
+      <c r="C38" s="155">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>250</v>
+      </c>
+      <c r="B40" s="116">
+        <f>'MODELO VALORACIÓN SIMPLIFICADO'!B81/'MODELO VALORACIÓN SIMPLIFICADO'!B48</f>
+        <v>0.81980486500935579</v>
+      </c>
+      <c r="C40" s="116">
+        <f ca="1">'MODELO VALORACIÓN SIMPLIFICADO'!C81/'MODELO VALORACIÓN SIMPLIFICADO'!C48</f>
+        <v>0.88823330251925392</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E9:E10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>